<commit_message>
thu commit at home
</commit_message>
<xml_diff>
--- a/src/main/dataProviderFiles/LoginData.xlsx
+++ b/src/main/dataProviderFiles/LoginData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -27,13 +28,40 @@
     <t>password</t>
   </si>
   <si>
-    <t>000350</t>
+    <t>afacctno</t>
+  </si>
+  <si>
+    <t>Cash. 046C000350 - cá nhân TN</t>
+  </si>
+  <si>
+    <t>Cash. 046FIA0016 - NDT NUOC NGOAI (cá nhân)</t>
   </si>
   <si>
     <t>046C000350</t>
   </si>
   <si>
-    <t>Timeout</t>
+    <t>046FIA0016</t>
+  </si>
+  <si>
+    <t>023C000350</t>
+  </si>
+  <si>
+    <t>notice</t>
+  </si>
+  <si>
+    <t>Tài khoản đăng nhập không hợp lệ!</t>
+  </si>
+  <si>
+    <t>Sai mật khẩu!</t>
+  </si>
+  <si>
+    <t>Chưa nhập Số tài khoản</t>
+  </si>
+  <si>
+    <t>Chưa nhập Mật khẩu</t>
+  </si>
+  <si>
+    <t>Chưa nhập Số tài khoảnChưa nhập Mật khẩu</t>
   </si>
 </sst>
 </file>
@@ -83,10 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,15 +400,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -388,29 +419,105 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>123</v>
       </c>
-      <c r="C2">
-        <v>30</v>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>123</v>
       </c>
-      <c r="C3">
-        <v>180</v>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="62.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>